<commit_message>
Added new logic for refresh and fixed the button alignments
</commit_message>
<xml_diff>
--- a/backend/translations.xlsx
+++ b/backend/translations.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1186,9 +1186,179 @@
         <v>weight.uguyut</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="str">
+        <v>English → Santhali</v>
+      </c>
+      <c r="C47" t="str">
+        <v>adada</v>
+      </c>
+      <c r="D47" t="str">
+        <v>ᱴᱟᱹᱯᱩ ᱨᱮ</v>
+      </c>
+      <c r="E47" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="str">
+        <v>English → Santhali</v>
+      </c>
+      <c r="C48" t="str">
+        <v>asas</v>
+      </c>
+      <c r="D48" t="str">
+        <v>ᱵᱮᱥ</v>
+      </c>
+      <c r="E48" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="str">
+        <v>English → Santhali</v>
+      </c>
+      <c r="C49" t="str">
+        <v>asasas</v>
+      </c>
+      <c r="D49" t="str">
+        <v>ᱟᱥᱟᱥᱟᱥ</v>
+      </c>
+      <c r="E49" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="str">
+        <v>English → Santhali</v>
+      </c>
+      <c r="C50" t="str">
+        <v>adadadad</v>
+      </c>
+      <c r="D50" t="str">
+        <v>ᱟᱰᱟᱰᱟᱰᱟᱰᱟ</v>
+      </c>
+      <c r="E50" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="str">
+        <v>English → Santhali</v>
+      </c>
+      <c r="C51" t="str">
+        <v>adadad</v>
+      </c>
+      <c r="D51" t="str">
+        <v>ᱵᱟᱵᱟ</v>
+      </c>
+      <c r="E51" t="str">
+        <v>ᱵᱟᱵᱟᱢᱢᱨ</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="str">
+        <v>English → Santhali</v>
+      </c>
+      <c r="C52" t="str">
+        <v>Prerna Pagal Hai</v>
+      </c>
+      <c r="D52" t="str">
+        <v>ᱯᱨᱮᱨᱱᱟ ᱫᱚ ᱯᱟᱜᱽᱞᱟ ᱜᱮᱭᱟᱭ</v>
+      </c>
+      <c r="E52" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="str">
+        <v>English → Santhali</v>
+      </c>
+      <c r="C53" t="str">
+        <v>Prerna is a good girl</v>
+      </c>
+      <c r="D53" t="str">
+        <v>ᱯᱨᱮᱨᱱᱟ ᱫᱚ ᱱᱟᱯᱟᱭ ᱠᱩᱲᱤ ᱠᱟᱱᱟᱭ</v>
+      </c>
+      <c r="E53" t="str">
+        <v>ᱯᱨᱮᱨᱱᱟ ᱫᱚ ᱱᱟᱯᱟᱭ ᱠᱩᱲᱤ ᱠᱟᱱᱟᱭᱢᱣᱤ</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="str">
+        <v>English → Santhali</v>
+      </c>
+      <c r="C54" t="str">
+        <v>Hi, My name is Nandu aka Nandani</v>
+      </c>
+      <c r="D54" t="str">
+        <v>ᱦᱟᱭ, ᱤᱧᱟᱜ ᱧᱩᱛᱩᱢ ᱫᱚ ᱱᱟᱱᱰᱩ ᱟᱨᱠᱟ ᱱᱟᱱᱰᱟᱱᱤ</v>
+      </c>
+      <c r="E54" t="str">
+        <v>ᱦᱟᱭ, ᱤᱧᱟᱜ ᱧᱩᱛᱩᱢ ᱫᱚ ᱱᱟᱱᱰᱩ ᱟᱨᱠᱟ ᱱᱟᱱᱰᱟᱱᱤᱠᱡᱢ</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="str">
+        <v>English → Santhali</v>
+      </c>
+      <c r="C55" t="str">
+        <v>adad</v>
+      </c>
+      <c r="D55" t="str">
+        <v>ᱵᱟᱵᱟ</v>
+      </c>
+      <c r="E55" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="str">
+        <v>Santhali → English</v>
+      </c>
+      <c r="C56" t="str">
+        <v>ᱣᱡᱧᱧ</v>
+      </c>
+      <c r="D56" t="str">
+        <v>Wjng</v>
+      </c>
+      <c r="E56" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E46"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E56"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>